<commit_message>
Cleaning up repo for submission
</commit_message>
<xml_diff>
--- a/Filtration project_Whale population and feeding information.xlsx
+++ b/Filtration project_Whale population and feeding information.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavoca/Documents/Research Data/Whale research/Prey consumption paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{116C0311-988D-3B43-9DDE-288D0A74A27B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE9B0E5-F16D-1041-B79A-8BFD00F80B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="560" windowWidth="27040" windowHeight="14340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="560" windowWidth="27040" windowHeight="14340" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IUCN 2019 Redlist" sheetId="5" r:id="rId1"/>
     <sheet name="B. musculus" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Precourt table" sheetId="6" r:id="rId3"/>
     <sheet name="B. physalus" sheetId="2" r:id="rId4"/>
     <sheet name="M. novaeangliae" sheetId="4" r:id="rId5"/>
     <sheet name="Resources" sheetId="3" r:id="rId6"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>IUCN population segments</t>
   </si>
@@ -327,13 +329,73 @@
   </si>
   <si>
     <t>Southern hemisphere historic estimate (Christensen 2006)</t>
+  </si>
+  <si>
+    <t>Common name</t>
+  </si>
+  <si>
+    <t>Scientific name</t>
+  </si>
+  <si>
+    <t>Pre-whaling abundance</t>
+  </si>
+  <si>
+    <t>Post-whaling abundance</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Percent decline</t>
+  </si>
+  <si>
+    <t>Balaenidae</t>
+  </si>
+  <si>
+    <t>Balaenopteridae</t>
+  </si>
+  <si>
+    <t>Blue whale</t>
+  </si>
+  <si>
+    <t>Fin whale</t>
+  </si>
+  <si>
+    <t>Humpback whale</t>
+  </si>
+  <si>
+    <t>Sei whale</t>
+  </si>
+  <si>
+    <t>Bryde's whale</t>
+  </si>
+  <si>
+    <t>Common minke whale</t>
+  </si>
+  <si>
+    <t>Antarctic minke whale</t>
+  </si>
+  <si>
+    <t>North Atlantic right whale</t>
+  </si>
+  <si>
+    <t>North Pacific right whale</t>
+  </si>
+  <si>
+    <t>Southern right whale</t>
+  </si>
+  <si>
+    <t>Bowhead whale</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -391,6 +453,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -400,10 +482,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -436,7 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,6 +553,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -810,9 +933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J2" sqref="J2:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1582,12 +1705,294 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7E5ECD-5C8A-304C-934B-71BBF1709546}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="8">
+        <v>376120</v>
+      </c>
+      <c r="E2" s="8">
+        <v>4727</v>
+      </c>
+      <c r="F2" s="11">
+        <f>(D2-E2)/D2*100</f>
+        <v>98.743220248856744</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="8">
+        <v>936000</v>
+      </c>
+      <c r="E3" s="8">
+        <v>109600</v>
+      </c>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F13" si="0">(D3-E3)/D3*100</f>
+        <v>88.290598290598282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="8">
+        <v>285400</v>
+      </c>
+      <c r="E4" s="8">
+        <v>42070</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="0"/>
+        <v>85.259285213735097</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="8">
+        <v>294400</v>
+      </c>
+      <c r="E5" s="8">
+        <v>49090</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>83.325407608695656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="8">
+        <v>190800</v>
+      </c>
+      <c r="E6" s="8">
+        <v>132400</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="0"/>
+        <v>30.607966457023061</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="8">
+        <v>344300</v>
+      </c>
+      <c r="E7" s="8">
+        <v>188900</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="0"/>
+        <v>45.135056636654078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="8">
+        <v>478000</v>
+      </c>
+      <c r="E8" s="8">
+        <v>318000</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="0"/>
+        <v>33.472803347280333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="8">
+        <v>27800</v>
+      </c>
+      <c r="E9" s="8">
+        <v>6740</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>75.755395683453244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="8">
+        <v>27800</v>
+      </c>
+      <c r="E10" s="8">
+        <v>368</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="0"/>
+        <v>98.676258992805757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="8">
+        <v>98300</v>
+      </c>
+      <c r="E11" s="8">
+        <v>368</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="0"/>
+        <v>99.625635808748726</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="8">
+        <v>114000</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9450</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="0"/>
+        <v>91.71052631578948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13">
+        <f>SUM(D2:D12)</f>
+        <v>3172920</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E2:E12)</f>
+        <v>861713</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="0"/>
+        <v>72.841641138131436</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>